<commit_message>
Removed read only functionality, it was screwing up openpyxl.
</commit_message>
<xml_diff>
--- a/test/BaobabMetadataTemplate.xlsx
+++ b/test/BaobabMetadataTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,11 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false"/>
+    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false">NA()</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet1"</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="Excel_BuiltIn_Print_Area" vbProcedure="false"/>
+    <definedName function="false" hidden="false" localSheetId="1" name="Excel_BuiltIn_Print_Area" vbProcedure="false">NA()</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet2"</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="Excel_BuiltIn_Print_Area" vbProcedure="false"/>
+    <definedName function="false" hidden="false" localSheetId="2" name="Excel_BuiltIn_Print_Area" vbProcedure="false">NA()</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet3"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -139,6 +139,7 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -230,31 +231,32 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8348214285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5446428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.1205357142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.9866071428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.6919642857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.2544642857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.1116071428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.1339285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.9776785714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1339285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.4241071428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="25.1116071428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="36.8035714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="29.53125"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="25.3973214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="19.2678571428571"/>
-    <col collapsed="false" hidden="false" max="256" min="19" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.1964285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.84375"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.71875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.4821428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.9776785714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8035714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6696428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.1651785714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="24.8035714285714"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="36.2633928571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="29.1741071428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="25.0401785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="19.0178571428571"/>
+    <col collapsed="false" hidden="false" max="257" min="19" style="1" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.97767857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +374,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -387,18 +389,19 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.97767857142857"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -413,18 +416,19 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.97767857142857"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>